<commit_message>
add plot count revenue
</commit_message>
<xml_diff>
--- a/database/macro/بودجه/my_budget.xlsx
+++ b/database/macro/بودجه/my_budget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="کسری بودجه" sheetId="4" r:id="rId1"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +903,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -2219,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -2680,7 +2680,7 @@
         <v>0.14624691815968205</v>
       </c>
       <c r="D15" s="17">
-        <f t="shared" si="5"/>
+        <f>D7/$G7</f>
         <v>4.5129866439466919E-2</v>
       </c>
       <c r="E15" s="17">
@@ -2789,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="A8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>